<commit_message>
added the BrandItemPageData  and BrandItemPage elements
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="144">
   <si>
     <t>URL</t>
   </si>
@@ -179,6 +179,299 @@
   </si>
   <si>
     <t>,https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars/,https://www.famous-smoke.com/cigar-brand-list/</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+ruby+cigars</t>
+  </si>
+  <si>
+    <t>1502 Ruby Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Ruby cigars are an artisan quality selection handcrafted in Estelí, Nicaragua. These aesthetically appealing cigars offer you a medium-full blend of...</t>
+  </si>
+  <si>
+    <t>1502 Ruby Cigars</t>
+  </si>
+  <si>
+    <t>1502 Ruby cigars are an artisan quality selection handcrafted in Estelí, Nicaragua. These aesthetically appealing cigars offer you a medium-full blend of the most select Nicaraguan Estelí &amp; Jalapa tobaccos BOX-PRESSED in an attractively dark, oily Cuban-seed wrapper grown in Ecuador. The smoke is exceptionally well-balanced, serving-up an earthy-woody flavor profile with notes of sweet cedar and toasted nuts. Try this real gem of a cigar by adding some to your cart today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Ruby Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1994+by+la+flor+dominicana+cigars</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana holds a very special meaning to the company that brought you some of the highest rated cigars year after year. The 1994...</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana Cigars</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana holds a very special meaning to the company that brought you some of the highest rated cigars year after year. The 1994 commemorates Litto and Ines Gomez's 20th year with the LFD cigar brand they created. Dominican longfillers and binders are dressed in an oily Mexican San Andres natural wrapper, with 4 sizes to choose from. If you're a fan of LFD, you should only expect yet another cigar with stellar flavor and a full bodied strength profile. Get yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All La Flor Dominicana Brands » 1994 By La Flor Dominicana Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/la+flor+dominicana+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/262+cigars</t>
+  </si>
+  <si>
+    <t>262 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 cigars for sale at Famous Smoke Shop's online cigar store. These boutique cigars present a revolution in premium cigar quality, taste, and complexity.</t>
+  </si>
+  <si>
+    <t>262 Cigars</t>
+  </si>
+  <si>
+    <t>The brainchild of Clint Aaron and Mike Justice, 262 Cigars is a collective of premium cigar brands that have been riding the new wave of boutique cigars into the marketplace since 2010. The name stands for February 1962, the month and year that President John F. Kennedy signed the Cuban Trade Embargo. It also stands for something more than just really good cigars; it stands for a new paradigm and an ideology to which Aaron and Justice have assigned the slogan, "Smoke the Revolution."
+No revolution would be complete without a manifesto, and the 262 Manifesto is a call to action for cigar smokers to band together and tell local, state, and federal government officials that they will not stand for excessive tobacco taxation and unconstitutional smoking bans. "I believe in the constitution and fully trust what the founders setup for us," says Mike Justice. "Our Ideologies are the foundations of how we live our lives, the decisions we make, and the people we associate with."
+Made in Honduras Paradigm cigars start with Nicaraguan Seco and Ligero tobaccos from Estelí and Jalapa, a Colombian Cuban-seed Cubito leaf, and a Honduran binder wrapped in a luscious Brazilian Mata Fina leaf that pulls everything together to deliver a creamy, complex, and medium-full smoke that exhibits notes of citrus, coffee, pepper, cedar, cocoa and sweet tobacco.
+Our Ideologies are what make us who we are, and 262 Ideology cigars represent the passion to create great cigars, the fortitude to transcend the opposition, and the resolve to smoke free. Using a mild 3-nation core blend rolled in flawless Nicaraguan Habano Rosado wrappers, the 262 Ideology will ring home with your palate and remind you what is was about cigars that made you fall in love with them. Their effortless draw offers a toasty, buttery, and creamy-smooth smoke that pledges to put your troubles on "hold" for a most relaxing experience.
+During the events leading up to our nation's revolution, Paul Revere was among those who answered the call for freedom with selfless courage, and made his mark on history. That passion is reflected in the 262 Revere cigars selection. If you love the bold taste of Nicaraguan puros, the Revere selection embraces a blend of long-fillers from Estelí, Condega, and Jalapa rolled in a glossy and naturally sweet-tasting Jalapa wrapper. The smoke is full-bodied, offering a multitude of floral and herbal notes with citrus peel, cocoa, and spice in the mix, making the 262 Revere a marvelous choice for lovers of the best Nicaraguan cigars.
+While all of the above brands have a cigar revolution theme, 262 Allegiance cigars takes a stronger tone. State by state, town by town, and at the Federal level, too, there is a growing opposition to our cigar culture, and it's time to take a side. So, in an effort to thwart those efforts, Clint Aaron has created a medium-bodied cigar that will appeal to cigar smokers at every level. Made in Estelí, Nicaragua, Allegiance marries Nicaraguan and Honduran long-fillers to an oily Brazilian Mata Fina wrapper for a satisfying smoke with an exotic mix of spice, citrus, and earthy flavors. If you want a cigar made with outstanding quality and taste, turn your allegiance to this selection.
+"</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 262 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+allegiance+cigars</t>
+  </si>
+  <si>
+    <t>262 Allegiance Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>I pledge allegiance to the cigar called 262 Allegiance. Originally planned as a seasonal blend, Allegiance was met with such an enthusiastic response the...</t>
+  </si>
+  <si>
+    <t>262 Allegiance Cigars</t>
+  </si>
+  <si>
+    <t>I pledge allegiance to the cigar called 262 Allegiance. Originally planned as a seasonal blend, Allegiance was met with such an enthusiastic response the company decided to make it a full production cigar handcrafted at Tabacalera Carreras factory in Esteli, Nicaragua with a Brazilian Mata Fina wrapper, Nicaraguan binder and a Honduran-Nicaraguan filler blend. Expect an effortless, enjoyable, and very affordable smoke that's mild to medium in body, yet very rich in flavor. Order yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Allegiance Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/262+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+ideology+cigars</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262...</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Ideology is Mild yet complex smoke with Nicaraguan, Mexican, and Dominican fillers, a Nicaraguan binder, and a Nicaraguan Habano Rosado wrapper that ads a buttery creaminess to an outstanding smoke. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Ideology Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+paradigm+cigars</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262...</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Paradigm is a medium to full bodied complex smoke with Nicaraguan and rare Colombian fillers, a Honduran binder, and a rich and creamy Brazilian Mata Fina wrapper. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Paradigm Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+revere+1+cigars</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is...</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Revere is a full bodied Nicaraguan Puro with a blend of fillers from Esteli, Jalapa, and Condega, a binder with Esteli and Jalapa tobaccos, and a Jalapa Valley wrapper. The result is a complex and bold cigar packed with unbelievable flavor. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Revere Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/4th+generation+pipe+accessories</t>
+  </si>
+  <si>
+    <t>4th Generation Pipe | Famous Smoke</t>
+  </si>
+  <si>
+    <t>4th Generation pipe accessories and tobacco say Stokkebye, so you know they’re good. Order now and treat your pipe to a rich selection of their best blends!</t>
+  </si>
+  <si>
+    <t>4th Generation Pipe</t>
+  </si>
+  <si>
+    <t>4th Generation pipe accessories and tobacco celebrate the rich history of Stokkebye tobacco – and fourth generation family head Erik Stokkebye has done the family proud with this rich variety of pipe tobaccos. Based on decades of his clan’s expertise that started with founding father Erik Peter, who began the tobacco journey in 1882 - this 4th Generation Stokkebye channels the legacy to offer to you a wide array of tastes, ranging from the mild and aromatic to mature Virginia. Order yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Accessories » Accessories » Tobacco Brand List » 4th Generation Pipe</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/accessories,https://www.famous-smoke.com/tobacco-brand-list</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/6+pack+samplers+cigars</t>
+  </si>
+  <si>
+    <t>6 Pack Cigar Samplers | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Sure, you're used to seeing cigars presented in 5-packs, but we've taken them one step beyond in this delicious series of 6-Packs presented in a wide...</t>
+  </si>
+  <si>
+    <t>6 Pack Cigar Samplers</t>
+  </si>
+  <si>
+    <t>Sure, you're used to seeing cigars presented in 5-packs, but we've taken them one step beyond in this delicious series of 6-Packs presented in a wide variety of strengths, wrappers, and even a couple of coffee flavored combos. Starring the bestselling cigars in the business at nice prices, now you can get a 6-pack without working out. Browse through the list now and order the Best Sellers 6-Packs that are right for you. There's no better or thriftier way to own great cigars!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » 6 Pack Cigar Samplers</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/601+cigars</t>
+  </si>
+  <si>
+    <t>601 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>601 Cigars is known within the industry as being some of the most delicious, well made, heavy hitting smokes around. Famous offers discount prices on 601 Cigars</t>
+  </si>
+  <si>
+    <t>601 Cigars</t>
+  </si>
+  <si>
+    <t>601 Cigars is known throughout the industry as being some of the most delicious, well made, heavy hitting stogies around. Making use of virtually every priming of numerous types of tobacco, Erik Espinosa along with then partner Eddie Ortega blended and released the 601 cigar line in the mid 2000s with the infamous Blue, Red, and Green labels. From there, the brand only kept expanding with the La Bomba and Warhead. Now you can have your own slice of stogie heaven with Famous Smoke Shop discount prices on all lines of this wonderful cigar. Get yours today from our massive inventory and save today!
+About 601 Cigars
+At the age of 3 months old, Erik Espinosa and his family moved to Miami in search of a more prosperous life. Of course, being only 3 months old, it was hard for him to find any work, but we all agree here that he had a lot of ambition to make such a drastic move at such a young age. As he got older, he adopted his passion for cigars from his father who worked in the industry, and in 1997 began his career in this highly competitive market. Gaining knowledge from leading cigar manufacturers such as Alec Bradley, Gurkha, Rocky Patel, and Drew Estate, Erik soaked in as much information as he could to learn every single detail he can to prepare himself when the time came that he would open his own factory.
+Finally, in 2004, Mr. Espinosa along with former partner Eddie Ortega, EO Brands was formed, and the 601 Cigars line was born with innovative new blends not seen in any other line before. They were one of the first companies to incorporate a Mexican San Andreas wrapper in their blends which started a massive trend in using this inexpensive and flavorful tobacco. For close to a decade, Erik Espinosa released new blends consistently, but he really hit his stride in 2012 with the birth of La Zona Premium Cigar Company. This gave him complete power to create even more blends on his own and re-release cigars he had made over at EO Brands.
+Now working with his son Erik Jr., Mr. Espinosa has had nothing but success reaching cigar lovers both young and old with 601 cigars being one of the main attractions. Lines like the 601 Blue Label and 601 Green label has been filling older cigar smoker’s humidors for over a decade now, with 601 La Bomba and Warhead appealing to a younger market of full strength, full bodied smokers. But no matter what a customer prefers, La Zona has a stogie to satisfy anyone’s craving.
+Now you can experience 601 Cigars at massively discounted prices made available through Famous Smoke Shop and its large inventory. Famous Smoke Shop holds the most cigars in stock through buying from each of it’s suppliers directly, ensuring you get the cigars you want in any size available. Get your 601 Cigars today from Famous and save money on these premium hand rolled stogies.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 601 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+accesories+and+samplers+cigars</t>
+  </si>
+  <si>
+    <t>601 Accesories And Cigar Samplers | Famous Smoke</t>
+  </si>
+  <si>
+    <t>601 cigars were originally created by Amilcar Perez-Castro in August of 2006, and have since taken off like wildfire. Now manufactured at Tavicusa S.A in...</t>
+  </si>
+  <si>
+    <t>601 Accesories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>601 cigars were originally created by Amilcar Perez-Castro in August of 2006, and have since taken off like wildfire. Now manufactured at Tavicusa S.A in Estelí, Nicaragua under the direction of Erik Espinosa, since its debut, the 601 series has received heaps of praise from cigar media and cigar smokers alike. Ranging from medium to full-bodied, the line offers something wonderful for even the most discerning palates. Try one of these supreme selections today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Accesories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/601+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+blue+label+cigars</t>
+  </si>
+  <si>
+    <t>601 Blue Label Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>The 601 'Blue' cigar series are slightly box-pressed, medium to full-bodied premium cigars. Manufactured by Tavicusa S.A., they boast an exquisite recipe...</t>
+  </si>
+  <si>
+    <t>601 Blue Label Cigars</t>
+  </si>
+  <si>
+    <t>The 601 'Blue' cigar series are slightly box-pressed, medium to full-bodied premium cigars. Manufactured by Tavicusa S.A., they boast an exquisite recipe of perfectly-aged Nicaraguan longfillers finished in a dark Nicaraguan Habano wrapper. Precisely blended to offer a rich, well-balanced medley of dark and naturally sweet tobacco flavors enhanced by an arousing aroma, if you prefer taste over strength, this is the 601 for you. Make sure you have a box on-hand for those special occasions.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Blue Label Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+green+label+oscuro+cigars</t>
+  </si>
+  <si>
+    <t>601 Green Label Oscuro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>The 601 'Green' cigar series comprises a full-bodied blend created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan long-filler...</t>
+  </si>
+  <si>
+    <t>601 Green Label Oscuro Cigars</t>
+  </si>
+  <si>
+    <t>The 601 'Green' cigar series comprises a full-bodied blend created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan long-filler tobaccos. Rolled in an exquisite Nicaraguan Habano Oscuro wrapper leaf, these puros are, by far, among the most full-flavored in the 601 series. Each cigar is precisely blended to offer a well-balanced, robust smoke brimming with juicy, complex flavors. If you crave big, bold flavor and aroma in your cigars, add a box to your cart now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Green Label Oscuro Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+la+bomba+1+cigars</t>
+  </si>
+  <si>
+    <t>601 La Bomba Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Calling this new addition to the highly-acclaimed 601 cigars selection The Bomb is an understatement. The blend consists of an all-Nicaraguan longfiller &amp;...</t>
+  </si>
+  <si>
+    <t>601 La Bomba Cigars</t>
+  </si>
+  <si>
+    <t>Calling this new addition to the highly-acclaimed 601 cigars selection The Bomb is an understatement. The blend consists of an all-Nicaraguan longfiller &amp; binder core rolled in a savory Habano wrapper leaf. If you love lots'a Ligero, you'll enjoy this explosive, extra-strength smoke in a Nicaraguan puro format. Presented in boxes of 10 cigars spanning several popular sizes, La Bomba is chock full of dark, spicy tobacco flavor. Order your box now (Experienced smokers preferred).</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 La Bomba Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+red+label+habano+cigars</t>
+  </si>
+  <si>
+    <t>601 Red Label Habano Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>601 Red Label cigars are full-bodied premium cigars created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan longfillers topped...</t>
+  </si>
+  <si>
+    <t>601 Red Label Habano Cigars</t>
+  </si>
+  <si>
+    <t>601 Red Label cigars are full-bodied premium cigars created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan longfillers topped with an attractively oily Nicaraguan Natural Habano wrapper. The 601 'Red' is blended for the experienced cigar smoker providing a stunning mosaic of well-balanced flavors, while maintaining its complex flavor profile from start to finish with an enticing aroma. If you love robust and peppery Nicaraguan puros, order a box or a 5-pack now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Red Label Habano Cigars</t>
   </si>
 </sst>
 </file>
@@ -195,7 +488,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +525,18 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -346,11 +649,47 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,6 +755,132 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -740,102 +1205,624 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="54.546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="54.546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="31.0078125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.48046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="71.23046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="71.23046875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="47.58203125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="145.84375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="32.0546875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="81.71875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="114.3515625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="126.45703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="178.8125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="10.87109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="44" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="45" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="46" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="57" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="H15" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="H17" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" s="60" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="61" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="62" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="62" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="H20" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="63" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="64" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="64" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="64" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="64" t="s">
+        <v>142</v>
+      </c>
+      <c r="G21" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="H21" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the wait and check of the TakeScreenshot interface
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="BrandItemPageData" r:id="rId8" sheetId="16"/>
-    <sheet name="BrandPageData" r:id="rId7" sheetId="17"/>
+    <sheet name="BrandItemPageData" r:id="rId8" sheetId="26"/>
+    <sheet name="BrandPageData" r:id="rId7" sheetId="27"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9969" uniqueCount="4329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11238" uniqueCount="4330">
   <si>
     <t>URL</t>
   </si>
@@ -17803,6 +17803,9 @@
   <si>
     <t>Arturo Fuente Seleccion D'Oro Cigars</t>
   </si>
+  <si>
+    <t>262 ALLEGIANCE ROBUSTO</t>
+  </si>
 </sst>
 </file>
 
@@ -17818,7 +17821,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -17915,8 +17918,58 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="70">
+  <borders count="110">
     <border>
       <left/>
       <right/>
@@ -18245,11 +18298,191 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="897">
+  <cellXfs count="1012">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -20937,6 +21170,351 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="73" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="77" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="81" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="85" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="89" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="93" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="97" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="101" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="101" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="105" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="105" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="105" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="109" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="109" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -21253,7 +21831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -21261,929 +21839,131 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="100.90625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="100.90625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="79.421875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="125.86328125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="33.21484375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="73.765625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="73.765625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="52.13671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="98.4296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5859375" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="255.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="185.734375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="248.50390625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="27.453125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="24.0859375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="113.5625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="166.87890625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.1796875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.69921875" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="13.95703125" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.87109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="862" t="s">
+      <c r="A1" s="1007" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="862" t="s">
+      <c r="B1" s="1007" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="862" t="s">
+      <c r="C1" s="1007" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="862" t="s">
+      <c r="D1" s="1007" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="862" t="s">
+      <c r="E1" s="1007" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="862" t="s">
+      <c r="F1" s="1007" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="862" t="s">
+      <c r="G1" s="1007" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="862" t="s">
+      <c r="H1" s="1007" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="862" t="s">
+      <c r="I1" s="1007" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="862" t="s">
+      <c r="J1" s="1007" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="862" t="s">
+      <c r="K1" s="1007" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="862" t="s">
+      <c r="L1" s="1007" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="863" t="s">
+      <c r="A2" s="1008" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="863" t="s">
+      <c r="B2" s="1008" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="863" t="s">
+      <c r="C2" s="1008" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="863" t="s">
+      <c r="D2" s="1008" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="863" t="s">
+      <c r="E2" s="1008" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="863" t="s">
+      <c r="F2" s="1008" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="863" t="s">
+      <c r="G2" s="1008" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="863" t="s">
+      <c r="H2" s="1008" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="863" t="s">
+      <c r="I2" s="1008" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="863" t="s">
+      <c r="J2" s="1008" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="863" t="s">
+      <c r="K2" s="1008" t="s">
         <v>268</v>
       </c>
-      <c r="L2" s="863" t="s">
+      <c r="L2" s="1008" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="864" t="s">
+      <c r="A3" s="1009" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="864" t="s">
+      <c r="B3" s="1009" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="864" t="s">
+      <c r="C3" s="1009" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="864" t="s">
+      <c r="D3" s="1009" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="864" t="s">
+      <c r="E3" s="1009" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="864" t="s">
+      <c r="F3" s="1009" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="864" t="s">
+      <c r="G3" s="1009" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="864" t="s">
+      <c r="H3" s="1009" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="864" t="s">
+      <c r="I3" s="1009" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="864" t="s">
+      <c r="J3" s="1009" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="864" t="s">
+      <c r="K3" s="1009" t="s">
         <v>268</v>
       </c>
-      <c r="L3" s="864" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="865" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="865" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="865" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="865" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="865" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="865" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="865" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="865" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="865" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="865" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="865" t="s">
-        <v>268</v>
-      </c>
-      <c r="L4" s="865" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="866" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="866" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="866" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="866" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="866" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="866" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="866" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="866" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="866" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="866" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="866" t="s">
-        <v>268</v>
-      </c>
-      <c r="L5" s="866" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="867" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="867" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="867" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="867" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="867" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="867" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="867" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="867" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" s="867" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="867" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" s="867" t="s">
-        <v>268</v>
-      </c>
-      <c r="L6" s="867" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="868" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="868" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="868" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="868" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="868" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="868" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="868" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="868" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="868" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" s="868" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" s="868" t="s">
-        <v>268</v>
-      </c>
-      <c r="L7" s="868" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="869" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="869" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="869" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="869" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="869" t="s">
-        <v>824</v>
-      </c>
-      <c r="F8" s="869" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="869" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="869" t="s">
-        <v>86</v>
-      </c>
-      <c r="I8" s="869" t="s">
-        <v>87</v>
-      </c>
-      <c r="J8" s="869" t="s">
-        <v>88</v>
-      </c>
-      <c r="K8" s="869" t="s">
-        <v>268</v>
-      </c>
-      <c r="L8" s="869" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="870" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="870" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="870" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="870" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="870" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="870" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="870" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" s="870" t="s">
-        <v>95</v>
-      </c>
-      <c r="I9" s="870" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="870" t="s">
-        <v>97</v>
-      </c>
-      <c r="K9" s="870" t="s">
-        <v>268</v>
-      </c>
-      <c r="L9" s="870" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="871" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="871" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="871" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="871" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="871" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="871" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="871" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="871" t="s">
-        <v>95</v>
-      </c>
-      <c r="I10" s="871" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="871" t="s">
-        <v>105</v>
-      </c>
-      <c r="K10" s="871" t="s">
-        <v>268</v>
-      </c>
-      <c r="L10" s="871" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="872" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="872" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="872" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="872" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" s="872" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="872" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" s="872" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" s="872" t="s">
-        <v>112</v>
-      </c>
-      <c r="I11" s="872" t="s">
-        <v>113</v>
-      </c>
-      <c r="J11" s="872" t="s">
-        <v>114</v>
-      </c>
-      <c r="K11" s="872" t="s">
-        <v>268</v>
-      </c>
-      <c r="L11" s="872" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="873" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="873" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="873" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="873" t="s">
-        <v>117</v>
-      </c>
-      <c r="E12" s="873" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="873" t="s">
-        <v>119</v>
-      </c>
-      <c r="G12" s="873" t="s">
-        <v>120</v>
-      </c>
-      <c r="H12" s="873" t="s">
-        <v>112</v>
-      </c>
-      <c r="I12" s="873" t="s">
-        <v>121</v>
-      </c>
-      <c r="J12" s="873" t="s">
-        <v>122</v>
-      </c>
-      <c r="K12" s="873" t="s">
-        <v>268</v>
-      </c>
-      <c r="L12" s="873" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="874" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="874" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="874" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="874" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="874" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="874" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="874" t="s">
-        <v>128</v>
-      </c>
-      <c r="H13" s="874" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" s="874" t="s">
-        <v>129</v>
-      </c>
-      <c r="J13" s="874" t="s">
-        <v>130</v>
-      </c>
-      <c r="K13" s="874" t="s">
-        <v>268</v>
-      </c>
-      <c r="L13" s="874" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="875" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="875" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" s="875" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="875" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="875" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="875" t="s">
-        <v>135</v>
-      </c>
-      <c r="G14" s="875" t="s">
-        <v>136</v>
-      </c>
-      <c r="H14" s="875" t="s">
-        <v>112</v>
-      </c>
-      <c r="I14" s="875" t="s">
-        <v>137</v>
-      </c>
-      <c r="J14" s="875" t="s">
-        <v>138</v>
-      </c>
-      <c r="K14" s="875" t="s">
-        <v>268</v>
-      </c>
-      <c r="L14" s="875" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="876" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="876" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="876" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="876" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="876" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="876" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="876" t="s">
-        <v>143</v>
-      </c>
-      <c r="H15" s="876" t="s">
-        <v>112</v>
-      </c>
-      <c r="I15" s="876" t="s">
-        <v>144</v>
-      </c>
-      <c r="J15" s="876" t="s">
-        <v>145</v>
-      </c>
-      <c r="K15" s="876" t="s">
-        <v>268</v>
-      </c>
-      <c r="L15" s="876" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="877" t="s">
-        <v>146</v>
-      </c>
-      <c r="B16" s="877" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="877" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="877" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="877" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="877" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="877" t="s">
-        <v>151</v>
-      </c>
-      <c r="H16" s="877" t="s">
-        <v>112</v>
-      </c>
-      <c r="I16" s="877" t="s">
-        <v>152</v>
-      </c>
-      <c r="J16" s="877" t="s">
-        <v>153</v>
-      </c>
-      <c r="K16" s="877" t="s">
-        <v>268</v>
-      </c>
-      <c r="L16" s="877" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="878" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="878" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" s="878" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="878" t="s">
-        <v>156</v>
-      </c>
-      <c r="E17" s="878" t="s">
-        <v>157</v>
-      </c>
-      <c r="F17" s="878" t="s">
-        <v>158</v>
-      </c>
-      <c r="G17" s="878" t="s">
-        <v>159</v>
-      </c>
-      <c r="H17" s="878" t="s">
-        <v>160</v>
-      </c>
-      <c r="I17" s="878" t="s">
-        <v>161</v>
-      </c>
-      <c r="J17" s="878" t="s">
-        <v>114</v>
-      </c>
-      <c r="K17" s="878" t="s">
-        <v>268</v>
-      </c>
-      <c r="L17" s="878" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="879" t="s">
-        <v>162</v>
-      </c>
-      <c r="B18" s="879" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="879" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="879" t="s">
-        <v>164</v>
-      </c>
-      <c r="E18" s="879" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="879" t="s">
-        <v>165</v>
-      </c>
-      <c r="G18" s="879" t="s">
-        <v>166</v>
-      </c>
-      <c r="H18" s="879" t="s">
-        <v>160</v>
-      </c>
-      <c r="I18" s="879" t="s">
-        <v>167</v>
-      </c>
-      <c r="J18" s="879" t="s">
-        <v>168</v>
-      </c>
-      <c r="K18" s="879" t="s">
-        <v>268</v>
-      </c>
-      <c r="L18" s="879" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="880" t="s">
-        <v>169</v>
-      </c>
-      <c r="B19" s="880" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" s="880" t="s">
-        <v>170</v>
-      </c>
-      <c r="D19" s="880" t="s">
-        <v>171</v>
-      </c>
-      <c r="E19" s="880" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="880" t="s">
-        <v>172</v>
-      </c>
-      <c r="G19" s="880" t="s">
-        <v>173</v>
-      </c>
-      <c r="H19" s="880" t="s">
-        <v>160</v>
-      </c>
-      <c r="I19" s="880" t="s">
-        <v>174</v>
-      </c>
-      <c r="J19" s="880" t="s">
-        <v>175</v>
-      </c>
-      <c r="K19" s="880" t="s">
-        <v>268</v>
-      </c>
-      <c r="L19" s="880" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="881" t="s">
-        <v>176</v>
-      </c>
-      <c r="B20" s="881" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="881" t="s">
-        <v>177</v>
-      </c>
-      <c r="D20" s="881" t="s">
-        <v>178</v>
-      </c>
-      <c r="E20" s="881" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="881" t="s">
-        <v>180</v>
-      </c>
-      <c r="G20" s="881" t="s">
-        <v>181</v>
-      </c>
-      <c r="H20" s="881" t="s">
-        <v>160</v>
-      </c>
-      <c r="I20" s="881" t="s">
-        <v>174</v>
-      </c>
-      <c r="J20" s="881" t="s">
-        <v>182</v>
-      </c>
-      <c r="K20" s="881" t="s">
-        <v>268</v>
-      </c>
-      <c r="L20" s="881" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="882" t="s">
-        <v>183</v>
-      </c>
-      <c r="B21" s="882" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="882" t="s">
-        <v>184</v>
-      </c>
-      <c r="D21" s="882" t="s">
-        <v>185</v>
-      </c>
-      <c r="E21" s="882" t="s">
-        <v>186</v>
-      </c>
-      <c r="F21" s="882" t="s">
-        <v>187</v>
-      </c>
-      <c r="G21" s="882" t="s">
-        <v>188</v>
-      </c>
-      <c r="H21" s="882" t="s">
-        <v>189</v>
-      </c>
-      <c r="I21" s="882" t="s">
-        <v>190</v>
-      </c>
-      <c r="J21" s="882" t="s">
-        <v>191</v>
-      </c>
-      <c r="K21" s="882" t="s">
-        <v>268</v>
-      </c>
-      <c r="L21" s="882" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="883" t="s">
-        <v>192</v>
-      </c>
-      <c r="B22" s="883" t="s">
-        <v>192</v>
-      </c>
-      <c r="C22" s="883" t="s">
-        <v>193</v>
-      </c>
-      <c r="D22" s="883" t="s">
-        <v>194</v>
-      </c>
-      <c r="E22" s="883" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="883" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="883" t="s">
-        <v>197</v>
-      </c>
-      <c r="H22" s="883" t="s">
-        <v>189</v>
-      </c>
-      <c r="I22" s="883" t="s">
-        <v>198</v>
-      </c>
-      <c r="J22" s="883" t="s">
-        <v>199</v>
-      </c>
-      <c r="K22" s="883" t="s">
-        <v>827</v>
-      </c>
-      <c r="L22" s="883" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="884" t="s">
-        <v>201</v>
-      </c>
-      <c r="B23" s="884" t="s">
-        <v>201</v>
-      </c>
-      <c r="C23" s="884" t="s">
-        <v>202</v>
-      </c>
-      <c r="D23" s="884" t="s">
-        <v>203</v>
-      </c>
-      <c r="E23" s="884" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="884" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="884" t="s">
-        <v>206</v>
-      </c>
-      <c r="H23" s="884" t="s">
-        <v>189</v>
-      </c>
-      <c r="I23" s="884" t="s">
-        <v>207</v>
-      </c>
-      <c r="J23" s="884" t="s">
-        <v>208</v>
-      </c>
-      <c r="K23" s="884" t="s">
-        <v>268</v>
-      </c>
-      <c r="L23" s="884" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="885" t="s">
-        <v>209</v>
-      </c>
-      <c r="B24" s="885" t="s">
-        <v>209</v>
-      </c>
-      <c r="C24" s="885" t="s">
-        <v>210</v>
-      </c>
-      <c r="D24" s="885" t="s">
-        <v>211</v>
-      </c>
-      <c r="E24" s="885" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="885" t="s">
-        <v>212</v>
-      </c>
-      <c r="G24" s="885" t="s">
-        <v>213</v>
-      </c>
-      <c r="H24" s="885" t="s">
-        <v>189</v>
-      </c>
-      <c r="I24" s="885" t="s">
-        <v>214</v>
-      </c>
-      <c r="J24" s="885" t="s">
-        <v>215</v>
-      </c>
-      <c r="K24" s="885" t="s">
-        <v>829</v>
-      </c>
-      <c r="L24" s="885" t="s">
+      <c r="L3" s="1009" t="s">
         <v>8</v>
       </c>
     </row>
@@ -22192,7 +21972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -22200,333 +21980,72 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="70.01171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="70.01171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="46.9609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="35.80078125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="54.546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="54.546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="31.0078125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="17.7265625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="126.45703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="178.8125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="81.71875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="112.65234375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="10.87109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="886" t="s">
+      <c r="A1" s="1010" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="886" t="s">
+      <c r="B1" s="1010" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="886" t="s">
+      <c r="C1" s="1010" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="886" t="s">
+      <c r="D1" s="1010" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="886" t="s">
+      <c r="E1" s="1010" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="886" t="s">
+      <c r="F1" s="1010" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="886" t="s">
+      <c r="G1" s="1010" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="886" t="s">
+      <c r="H1" s="1010" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="886" t="s">
+      <c r="I1" s="1010" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="887" t="s">
+      <c r="A2" s="1011" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="887" t="s">
+      <c r="B2" s="1011" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="887" t="s">
+      <c r="C2" s="1011" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="887" t="s">
+      <c r="D2" s="1011" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="887" t="s">
+      <c r="E2" s="1011" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="887" t="s">
+      <c r="F2" s="1011" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="887" t="s">
+      <c r="G2" s="1011" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="887" t="s">
+      <c r="H2" s="1011" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="887" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="888" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="888" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="888" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="888" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="888" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="888" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="888" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="888" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="888" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="889" t="s">
-        <v>217</v>
-      </c>
-      <c r="B4" s="889" t="s">
-        <v>217</v>
-      </c>
-      <c r="C4" s="889" t="s">
-        <v>218</v>
-      </c>
-      <c r="D4" s="889" t="s">
-        <v>219</v>
-      </c>
-      <c r="E4" s="889" t="s">
-        <v>220</v>
-      </c>
-      <c r="F4" s="889" t="s">
-        <v>221</v>
-      </c>
-      <c r="G4" s="889" t="s">
-        <v>222</v>
-      </c>
-      <c r="H4" s="889" t="s">
-        <v>223</v>
-      </c>
-      <c r="I4" s="889" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="890" t="s">
-        <v>224</v>
-      </c>
-      <c r="B5" s="890" t="s">
-        <v>224</v>
-      </c>
-      <c r="C5" s="890" t="s">
-        <v>225</v>
-      </c>
-      <c r="D5" s="890" t="s">
-        <v>226</v>
-      </c>
-      <c r="E5" s="890" t="s">
-        <v>227</v>
-      </c>
-      <c r="F5" s="890" t="s">
-        <v>228</v>
-      </c>
-      <c r="G5" s="890" t="s">
-        <v>229</v>
-      </c>
-      <c r="H5" s="890" t="s">
-        <v>223</v>
-      </c>
-      <c r="I5" s="890" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="891" t="s">
-        <v>230</v>
-      </c>
-      <c r="B6" s="891" t="s">
-        <v>230</v>
-      </c>
-      <c r="C6" s="891" t="s">
-        <v>231</v>
-      </c>
-      <c r="D6" s="891" t="s">
-        <v>232</v>
-      </c>
-      <c r="E6" s="891" t="s">
-        <v>233</v>
-      </c>
-      <c r="F6" s="891" t="s">
-        <v>234</v>
-      </c>
-      <c r="G6" s="891" t="s">
-        <v>235</v>
-      </c>
-      <c r="H6" s="891" t="s">
-        <v>223</v>
-      </c>
-      <c r="I6" s="891" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="892" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" s="892" t="s">
-        <v>236</v>
-      </c>
-      <c r="C7" s="892" t="s">
-        <v>237</v>
-      </c>
-      <c r="D7" s="892" t="s">
-        <v>238</v>
-      </c>
-      <c r="E7" s="892" t="s">
-        <v>239</v>
-      </c>
-      <c r="F7" s="892" t="s">
-        <v>240</v>
-      </c>
-      <c r="G7" s="892" t="s">
-        <v>241</v>
-      </c>
-      <c r="H7" s="892" t="s">
-        <v>223</v>
-      </c>
-      <c r="I7" s="892" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="893" t="s">
-        <v>242</v>
-      </c>
-      <c r="B8" s="893" t="s">
-        <v>242</v>
-      </c>
-      <c r="C8" s="893" t="s">
-        <v>243</v>
-      </c>
-      <c r="D8" s="893" t="s">
-        <v>244</v>
-      </c>
-      <c r="E8" s="893" t="s">
-        <v>245</v>
-      </c>
-      <c r="F8" s="893" t="s">
-        <v>246</v>
-      </c>
-      <c r="G8" s="893" t="s">
-        <v>247</v>
-      </c>
-      <c r="H8" s="893" t="s">
-        <v>248</v>
-      </c>
-      <c r="I8" s="893" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="894" t="s">
-        <v>249</v>
-      </c>
-      <c r="B9" s="894" t="s">
-        <v>249</v>
-      </c>
-      <c r="C9" s="894" t="s">
-        <v>250</v>
-      </c>
-      <c r="D9" s="894" t="s">
-        <v>251</v>
-      </c>
-      <c r="E9" s="894" t="s">
-        <v>252</v>
-      </c>
-      <c r="F9" s="894" t="s">
-        <v>253</v>
-      </c>
-      <c r="G9" s="894" t="s">
-        <v>254</v>
-      </c>
-      <c r="H9" s="894" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="894" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="895" t="s">
-        <v>255</v>
-      </c>
-      <c r="B10" s="895" t="s">
-        <v>255</v>
-      </c>
-      <c r="C10" s="895" t="s">
-        <v>256</v>
-      </c>
-      <c r="D10" s="895" t="s">
-        <v>257</v>
-      </c>
-      <c r="E10" s="895" t="s">
-        <v>258</v>
-      </c>
-      <c r="F10" s="895" t="s">
-        <v>259</v>
-      </c>
-      <c r="G10" s="895" t="s">
-        <v>260</v>
-      </c>
-      <c r="H10" s="895" t="s">
-        <v>261</v>
-      </c>
-      <c r="I10" s="895" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="896" t="s">
-        <v>262</v>
-      </c>
-      <c r="B11" s="896" t="s">
-        <v>262</v>
-      </c>
-      <c r="C11" s="896" t="s">
-        <v>263</v>
-      </c>
-      <c r="D11" s="896" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="896" t="s">
-        <v>265</v>
-      </c>
-      <c r="F11" s="896" t="s">
-        <v>266</v>
-      </c>
-      <c r="G11" s="896" t="s">
-        <v>267</v>
-      </c>
-      <c r="H11" s="896" t="s">
-        <v>261</v>
-      </c>
-      <c r="I11" s="896" t="s">
+      <c r="I2" s="1011" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed the item crawling action
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="BrandItemPageData" r:id="rId8" sheetId="34"/>
     <sheet name="BrandPageData" r:id="rId7" sheetId="35"/>
+    <sheet name="BrandItemPageData" r:id="rId8" sheetId="36"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14970" uniqueCount="7345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15006" uniqueCount="7347">
   <si>
     <t>URL</t>
   </si>
@@ -23184,6 +23184,12 @@
   </si>
   <si>
     <t>262 IDEOLOGY CIGARS FOR SALE</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » # Famous Cigars for Sale » # Famous Petite Corona Cigars - Natural</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » # Famous Cigars for Sale » # Famous Toro Cigars - Natural</t>
   </si>
 </sst>
 </file>
@@ -23208,7 +23214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -23280,8 +23286,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="47">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -23517,12 +23528,30 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1655">
+  <cellXfs count="1658">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -28484,6 +28513,15 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="50" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -28801,147 +28839,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="73.765625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="73.765625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="52.13671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="98.4296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5859375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="255.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="113.5625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="166.87890625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="24.1796875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.69921875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.95703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.87109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="252" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="252" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="252" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="252" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="252" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="252" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="252" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="252" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="252" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="252" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="252" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="252" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="253" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="253" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="253" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="253" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="253" t="s">
-        <v>1267</v>
-      </c>
-      <c r="F2" s="253" t="s">
-        <v>1268</v>
-      </c>
-      <c r="G2" s="253" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="253" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="253" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="253" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="253" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="253" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="254" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="254" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="254" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="254" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="254" t="s">
-        <v>1269</v>
-      </c>
-      <c r="F3" s="254" t="s">
-        <v>1270</v>
-      </c>
-      <c r="G3" s="254" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="254" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="254" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="254" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="254" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="254" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
@@ -28950,15 +28847,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="70.01171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="70.01171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="54.21875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="44.7421875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="126.45703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="178.8125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="10.87109375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="70.01171875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.01171875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="54.21875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="145.83984375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="44.7421875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="255.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="126.45703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="178.8125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.87109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -29283,4 +29180,145 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="73.765625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="73.765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="52.13671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="98.4296875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="25.5859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="126.71484375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="166.87890625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="24.1796875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="13.69921875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.95703125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="10.87109375" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1655" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1655" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1655" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1655" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1655" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1655" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1655" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1655" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1655" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1655" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1655" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1655" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1656" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1656" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1656" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1656" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1656" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F2" s="1656" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G2" s="1656" t="s">
+        <v>7345</v>
+      </c>
+      <c r="H2" s="1656" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1656" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1656" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1656" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="1656" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1657" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1657" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1657" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1657" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1657" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F3" s="1657" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G3" s="1657" t="s">
+        <v>7346</v>
+      </c>
+      <c r="H3" s="1657" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1657" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1657" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1657" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="1657" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added the items processing features
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="BrandPageData" r:id="rId7" sheetId="35"/>
-    <sheet name="BrandItemPageData" r:id="rId8" sheetId="36"/>
+    <sheet name="BrandItemPageData" r:id="rId8" sheetId="38"/>
+    <sheet name="BrandPageData" r:id="rId7" sheetId="39"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15006" uniqueCount="7347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15282" uniqueCount="7380">
   <si>
     <t>URL</t>
   </si>
@@ -23190,6 +23190,172 @@
   </si>
   <si>
     <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » # Famous Cigars for Sale » # Famous Toro Cigars - Natural</t>
+  </si>
+  <si>
+    <t># Famous Petite Corona</t>
+  </si>
+  <si>
+    <t># Famous Petite Corona
+This refillable vacuum-sealed humidor jar is stuffed with 36 #Famous Petite Corona cigars teeming with honeyed aromas of vanilla, sweet-creamy coffee, caramel, and toffee. Expect a mild, toothsome treat that beats many other flavor-infused cigars on both quality &amp; price, hands-down! #ordernow
+Full Specifications
+Strength:Mild
+Shape:Petite Corona
+Size:4 x 38
+Country:Nicaragua
+Wrapper Color:Natural
+Wrapper Origin:Honduran
+Wrapper Leaf:Connecticut
+Flavor:Infused</t>
+  </si>
+  <si>
+    <t>Country:Nicaragua,Strength:Mild,Wrapper Color:Natural,Shape:Petite Corona,Wrapper Origin:Honduran,Flavor:Infused,Size:4 x 38,Wrapper Leaf:Connecticut</t>
+  </si>
+  <si>
+    <t>NR consumer rating</t>
+  </si>
+  <si>
+    <t># Famous Toro</t>
+  </si>
+  <si>
+    <t># Famous Toro
+#Famous Toro cigars are mild, flavor-infused cigars ready to blow your mind with aromas of vanilla, toffee, caramel, and sweet-creamy coffee at a LOW Famous price. Plus, you can use the refillable vacuum-sealed humidor jar to keep your other favorite cigars fresh &amp; safe. Order yours now.
+Full Specifications
+Strength:Mild
+Shape:Toro
+Size:6 x 50
+Country:Nicaragua
+Wrapper Color:Natural
+Wrapper Origin:Honduran
+Wrapper Leaf:Connecticut
+Flavor:Infused</t>
+  </si>
+  <si>
+    <t>Country:Nicaragua,Strength:Mild,Size:6 x 50,Wrapper Color:Natural,Wrapper Origin:Honduran,Flavor:Infused,Shape:Toro,Wrapper Leaf:Connecticut</t>
+  </si>
+  <si>
+    <t>1502 Black Gold Toro</t>
+  </si>
+  <si>
+    <t>1502 Black Gold Toro
+1502 Black Gold Toro cigars are made for the cigar smoker who craves hearty tobacco flavor. The blend combines full-bodied Nicaraguan tobaccos with a spicy sun-grown maduro wrapper for a well-balanced, high-test smoke that sets a multitude of dark, peppery flavors in motion. Order your box today.
+Full Specifications
+Strength:Full
+Shape:Toro
+Size:6 x 50
+Country:Nicaragua
+Wrapper Color:Maduro
+Wrapper Origin:Not Available
+Wrapper Leaf:Sun Grown</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Black Gold Cigars for Sale » 1502 Black Gold Toro Cigars - Maduro</t>
+  </si>
+  <si>
+    <t>Country:Nicaragua,Strength:Full,Size:6 x 50,Shape:Toro,Wrapper Leaf:Sun Grown,Wrapper Origin:Not Available,Wrapper Color:Maduro</t>
+  </si>
+  <si>
+    <t>$118.95 $190.00 On Sale
+37% OFF</t>
+  </si>
+  <si>
+    <t>1502 Emerald Toro</t>
+  </si>
+  <si>
+    <t>1502 Emerald Toro
+1502 Emerald Toro cigars present a well-balanced, multi-layered smoke with superb construction and flavor. Flawless Nicaraguan Corojo wrappers cap a perfectly-balanced blend of Nicaraguan &amp; Mexican tobaccos that reveal notes of fruit, wood, spice, and a honeyed aroma. Drop a box in your cart now.
+Full Specifications
+Strength:Medium
+Shape:Toro
+Size:6 x 50
+Country:Nicaragua
+Wrapper Color:Natural
+Wrapper Origin:Nicaraguan
+Wrapper Leaf:Corojo</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Emerald Cigars for Sale » 1502 Emerald Toro Cigars - Natural</t>
+  </si>
+  <si>
+    <t>Country:Nicaragua,Wrapper Origin:Nicaraguan,Wrapper Leaf:Corojo,Strength:Medium,Size:6 x 50,Wrapper Color:Natural,Shape:Toro</t>
+  </si>
+  <si>
+    <t>$102.95 $152.00 On Sale
+32% OFF</t>
+  </si>
+  <si>
+    <t>1502 Emerald Torpedp 5 Pack</t>
+  </si>
+  <si>
+    <t>1502 Emerald Torpedp 5 Pack
+1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery Nicaragua Corojo wrappers that cap a carefully selected blend of Mexican San Andres long-fillers, plus Nicaraguan Estelí &amp; Condega tobaccos. Velvety smoke reveals delicate apple and other citrusy elements, plus a dash of sweet cedar, as the aroma lends fragrances of honey, vanilla and floral notes. Order some of these fine cigars today!
+Full Specifications
+Strength:Medium
+Shape:Torpedo
+Size:6 1/2 x 52
+Country:Nicaragua
+Wrapper Color:Natural
+Wrapper Origin:Nicaraguan
+Wrapper Leaf:Corojo</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Emerald Cigars for Sale » 1502 Emerald Torpedp Cigars - Natural</t>
+  </si>
+  <si>
+    <t>Country:Nicaragua,Wrapper Origin:Nicaraguan,Wrapper Leaf:Corojo,Strength:Medium,Wrapper Color:Natural,Shape:Torpedo,Size:6 1/2 x 52</t>
+  </si>
+  <si>
+    <t>$26.95 $40.00 On Sale
+33% OFF</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua Robusto 5 Pack</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua Robusto 5 Pack
+1502 Nicaragua cigars are super-premium, boutique selection from Nicaragua. Medium-full in body, these BOX-PRESSED puros boast master-level craftsmanship using a blend of perfectly-aged long-filler tobaccos from Esteli, Condega, Jalapa, and Ometepe. Expect a velvety smooth, medium-full smoke multi-layered with fruity, nutty and floral notes, plus a dash of Ometepe spice, enhanced by aromas of honey and vanilla. Reasonably-priced, too. Try these distinctive cigars by ordering some today.
+Full Specifications
+Strength:Medium
+Shape:Robusto
+Size:5 x 50
+Country:Nicaragua
+Wrapper Color:Natural
+Wrapper Origin:Nicaraguan
+Wrapper Leaf:Not Available</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Nicaragua Cigars for Sale » 1502 Nicaragua Robusto Cigars - Natural</t>
+  </si>
+  <si>
+    <t>Country:Nicaragua,Wrapper Origin:Nicaraguan,Strength:Medium,Wrapper Color:Natural,Wrapper Leaf:Not Available,Size:5 x 50,Shape:Robusto</t>
+  </si>
+  <si>
+    <t>$21.95 $32.50 On Sale
+32% OFF</t>
+  </si>
+  <si>
+    <t># Famous Cigars for Sale</t>
+  </si>
+  <si>
+    <t>1502 Cigars for Sale</t>
+  </si>
+  <si>
+    <t>1502 cigars are ready to take their place alongside many of the best Nicaraguan cigars you can buy. Presented in a variety of meticulously handcrafted blends that appeal to cigar smokers of every experience, these boutique cigars offer superb quality and taste in a limited number of box-pressed sizes in four savory selections. At the heart of the 1502 brand are the three core lines: the 1502 Emerald, 1502 Ruby, and 1502 Black Gold. Each cigar is unique in character and designed to be enjoyed morning, noon, and night, starting with the medium-bodied Emerald, followed by the more full-flavored Ruby, and concluding with the full-bodied Black Gold. Of course, the choice is yours as to when you choose to revel in their rich Nicaraguan flavor, but whichever 1502 cigar you buy, you're in for a truly satisfying and unforgettable experience.
+Launched in 2012 by native Nicaraguan, Enrique Sanchez Icaza, founder and CEO of Global Premium Cigars, 1502 Cigars were given their numerical name to commemorate the year Christopher Columbus discovered Nicaragua. Upon his arrival, Columbus also discovered a new world full of riches such as gold, silver, and precious stones for which the 1502 Emerald, Ruby, and Black Gold selections are named. But most importantly was the discovery of tobacco, which was used as a high value form of trade currency virtually equal to that of the Spanish Doubloon.
+"In our premium brand 1502, you will find three tobacco lines with the highest quality, where the sowing process, harvest, curing, aging and selection of each tobacco leaf is our major concern," says Señor Sanchez. "It takes more than five years, from the time the seeds are sown until the time you can enjoy one of our fine cigars; this is why patience is one of our greatest virtues in the art of tobacco production."
+1502 Emerald cigars yield a subtle strength and velvety smooth flavor that is achieved by a blend of long fillers from Estelí, Condega, and Mexico's San Andres valley pressed in a mouthwatering Nicaraguan Corojo Habano wrapper leaf. Delicate flavors of citrus, cedar, and roasted nut form the base, as aromas of honey, vanilla and floral notes drift amid the thick, creamy smoke.
+1502 Ruby cigars were created to delight discerning smokers who seek more body and complexity from their cigars. A lusciously dark Ecuadorian wrapper surrounds a well-balanced blend of fully-aged tobaccos from Estelí and Jalapa, for a medium-bodied, full-flavored smoke brimming with earthy elements, sweet cedar, and subtle hints of macadamia nuts and sunflower seeds.
+1502 Black Gold cigars bring on the muscle, full-tilt, for cigar smokers who enjoy extra bold tobacco flavor from end-to-end. A diverse Nicaraguan core is bound in two additional leaves, and finished in a maduro wrapper that's been nurtured by the sun to achieve the peak of flavor. Earthy-woody flavors abound as a layer of chili pepper works its way in, complemented by a delicate, chocolatey-fruity sweetness for a resounding multidimensional smoke.
+1502 Nicaragua cigars boast an "all-inclusive" Nicaraguan blend that uses tobaccos from Nicaragua's four main growing regions: Estelí, Jalapa, Condega, and Ometepe. Medium-full in body, this cigar's flavor profile fits somewhere between the 1502 Emerald and 1502 Ruby offering a velvety smoothness and amazing balance. The smoke is earthy and woody with some fruity elements, enhanced by a toasty, honeyed aroma.
+With so many wonderful blends to choose from, there's a 1502 cigar in your future. Browse the selections and find the 1502 cigar that's right for you – right now!</t>
+  </si>
+  <si>
+    <t>1502 Black Gold Cigars for Sale</t>
+  </si>
+  <si>
+    <t>1502 Emerald Cigars for Sale</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua Cigars for Sale</t>
   </si>
 </sst>
 </file>
@@ -23214,7 +23380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -23291,8 +23457,28 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="51">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -23546,12 +23732,84 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1658">
+  <cellXfs count="1684">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -28522,6 +28780,84 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="54" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="58" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="62" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="66" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -28839,7 +29175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -28847,333 +29183,283 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="70.01171875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.01171875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="54.21875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="145.83984375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="44.7421875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="79.203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="79.203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="52.48046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="105.15625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="28.93359375" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="255.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="126.45703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="178.8125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.87109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="148.59765625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="224.73828125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="141.6796875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.59765625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.87109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1644" t="s">
+      <c r="A1" s="1671" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1644" t="s">
+      <c r="B1" s="1671" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1644" t="s">
+      <c r="C1" s="1671" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1644" t="s">
+      <c r="D1" s="1671" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1644" t="s">
-        <v>26</v>
+      <c r="E1" s="1671" t="s">
+        <v>9</v>
       </c>
-      <c r="F1" s="1644" t="s">
+      <c r="F1" s="1671" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1644" t="s">
+      <c r="G1" s="1671" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1644" t="s">
+      <c r="H1" s="1671" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1644" t="s">
+      <c r="I1" s="1671" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1671" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1671" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1671" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1645" t="s">
-        <v>27</v>
+      <c r="A2" s="1672" t="s">
+        <v>13</v>
       </c>
-      <c r="B2" s="1645" t="s">
-        <v>27</v>
+      <c r="B2" s="1672" t="s">
+        <v>13</v>
       </c>
-      <c r="C2" s="1645" t="s">
-        <v>7329</v>
+      <c r="C2" s="1672" t="s">
+        <v>14</v>
       </c>
-      <c r="D2" s="1645" t="s">
-        <v>29</v>
+      <c r="D2" s="1672" t="s">
+        <v>15</v>
       </c>
-      <c r="E2" s="1645" t="s">
-        <v>7330</v>
+      <c r="E2" s="1672" t="s">
+        <v>7347</v>
       </c>
-      <c r="F2" s="1645" t="s">
-        <v>31</v>
+      <c r="F2" s="1672" t="s">
+        <v>7348</v>
       </c>
-      <c r="G2" s="1645" t="s">
-        <v>32</v>
+      <c r="G2" s="1672" t="s">
+        <v>7345</v>
       </c>
-      <c r="H2" s="1645" t="s">
-        <v>33</v>
+      <c r="H2" s="1672" t="s">
+        <v>17</v>
       </c>
-      <c r="I2" s="1645" t="s">
+      <c r="I2" s="1672" t="s">
+        <v>7349</v>
+      </c>
+      <c r="J2" s="1672" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1672" t="s">
+        <v>7350</v>
+      </c>
+      <c r="L2" s="1672" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1646" t="s">
-        <v>34</v>
+      <c r="A3" s="1673" t="s">
+        <v>20</v>
       </c>
-      <c r="B3" s="1646" t="s">
-        <v>34</v>
+      <c r="B3" s="1673" t="s">
+        <v>20</v>
       </c>
-      <c r="C3" s="1646" t="s">
-        <v>35</v>
+      <c r="C3" s="1673" t="s">
+        <v>21</v>
       </c>
-      <c r="D3" s="1646" t="s">
-        <v>36</v>
+      <c r="D3" s="1673" t="s">
+        <v>22</v>
       </c>
-      <c r="E3" s="1646" t="s">
-        <v>37</v>
+      <c r="E3" s="1673" t="s">
+        <v>7351</v>
       </c>
-      <c r="F3" s="1646" t="s">
-        <v>38</v>
+      <c r="F3" s="1673" t="s">
+        <v>7352</v>
       </c>
-      <c r="G3" s="1646" t="s">
-        <v>39</v>
+      <c r="G3" s="1673" t="s">
+        <v>7346</v>
       </c>
-      <c r="H3" s="1646" t="s">
-        <v>33</v>
+      <c r="H3" s="1673" t="s">
+        <v>17</v>
       </c>
-      <c r="I3" s="1646" t="s">
-        <v>41</v>
+      <c r="I3" s="1673" t="s">
+        <v>7353</v>
+      </c>
+      <c r="J3" s="1673" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1673" t="s">
+        <v>7350</v>
+      </c>
+      <c r="L3" s="1673" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1647" t="s">
-        <v>47</v>
+      <c r="A4" s="1674" t="s">
+        <v>1271</v>
       </c>
-      <c r="B4" s="1647" t="s">
-        <v>47</v>
+      <c r="B4" s="1674" t="s">
+        <v>1271</v>
       </c>
-      <c r="C4" s="1647" t="s">
-        <v>7331</v>
+      <c r="C4" s="1674" t="s">
+        <v>1272</v>
       </c>
-      <c r="D4" s="1647" t="s">
-        <v>49</v>
+      <c r="D4" s="1674" t="s">
+        <v>1273</v>
       </c>
-      <c r="E4" s="1647" t="s">
-        <v>7332</v>
+      <c r="E4" s="1674" t="s">
+        <v>7354</v>
       </c>
-      <c r="F4" s="1647" t="s">
-        <v>51</v>
+      <c r="F4" s="1674" t="s">
+        <v>7355</v>
       </c>
-      <c r="G4" s="1647" t="s">
-        <v>52</v>
+      <c r="G4" s="1674" t="s">
+        <v>7356</v>
       </c>
-      <c r="H4" s="1647" t="s">
-        <v>53</v>
+      <c r="H4" s="1674" t="s">
+        <v>1276</v>
       </c>
-      <c r="I4" s="1647" t="s">
+      <c r="I4" s="1674" t="s">
+        <v>7357</v>
+      </c>
+      <c r="J4" s="1674" t="s">
+        <v>7358</v>
+      </c>
+      <c r="K4" s="1674" t="s">
+        <v>7350</v>
+      </c>
+      <c r="L4" s="1674" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1648" t="s">
-        <v>54</v>
+      <c r="A5" s="1675" t="s">
+        <v>1287</v>
       </c>
-      <c r="B5" s="1648" t="s">
-        <v>54</v>
+      <c r="B5" s="1675" t="s">
+        <v>1287</v>
       </c>
-      <c r="C5" s="1648" t="s">
-        <v>7333</v>
+      <c r="C5" s="1675" t="s">
+        <v>1288</v>
       </c>
-      <c r="D5" s="1648" t="s">
-        <v>56</v>
+      <c r="D5" s="1675" t="s">
+        <v>1289</v>
       </c>
-      <c r="E5" s="1648" t="s">
-        <v>7334</v>
+      <c r="E5" s="1675" t="s">
+        <v>7359</v>
       </c>
-      <c r="F5" s="1648" t="s">
-        <v>58</v>
+      <c r="F5" s="1675" t="s">
+        <v>7360</v>
       </c>
-      <c r="G5" s="1648" t="s">
-        <v>59</v>
+      <c r="G5" s="1675" t="s">
+        <v>7361</v>
       </c>
-      <c r="H5" s="1648" t="s">
-        <v>53</v>
+      <c r="H5" s="1675" t="s">
+        <v>1293</v>
       </c>
-      <c r="I5" s="1648" t="s">
+      <c r="I5" s="1675" t="s">
+        <v>7362</v>
+      </c>
+      <c r="J5" s="1675" t="s">
+        <v>7363</v>
+      </c>
+      <c r="K5" s="1675" t="s">
+        <v>7350</v>
+      </c>
+      <c r="L5" s="1675" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1649" t="s">
-        <v>60</v>
+      <c r="A6" s="1676" t="s">
+        <v>1296</v>
       </c>
-      <c r="B6" s="1649" t="s">
-        <v>60</v>
+      <c r="B6" s="1676" t="s">
+        <v>1296</v>
       </c>
-      <c r="C6" s="1649" t="s">
-        <v>7335</v>
+      <c r="C6" s="1676" t="s">
+        <v>1297</v>
       </c>
-      <c r="D6" s="1649" t="s">
-        <v>62</v>
+      <c r="D6" s="1676" t="s">
+        <v>1298</v>
       </c>
-      <c r="E6" s="1649" t="s">
-        <v>7336</v>
+      <c r="E6" s="1676" t="s">
+        <v>7364</v>
       </c>
-      <c r="F6" s="1649" t="s">
-        <v>64</v>
+      <c r="F6" s="1676" t="s">
+        <v>7365</v>
       </c>
-      <c r="G6" s="1649" t="s">
-        <v>65</v>
+      <c r="G6" s="1676" t="s">
+        <v>7366</v>
       </c>
-      <c r="H6" s="1649" t="s">
-        <v>53</v>
+      <c r="H6" s="1676" t="s">
+        <v>1293</v>
       </c>
-      <c r="I6" s="1649" t="s">
+      <c r="I6" s="1676" t="s">
+        <v>7367</v>
+      </c>
+      <c r="J6" s="1676" t="s">
+        <v>7368</v>
+      </c>
+      <c r="K6" s="1676" t="s">
+        <v>7350</v>
+      </c>
+      <c r="L6" s="1676" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1650" t="s">
-        <v>66</v>
+      <c r="A7" s="1677" t="s">
+        <v>1304</v>
       </c>
-      <c r="B7" s="1650" t="s">
-        <v>66</v>
+      <c r="B7" s="1677" t="s">
+        <v>1304</v>
       </c>
-      <c r="C7" s="1650" t="s">
-        <v>7337</v>
+      <c r="C7" s="1677" t="s">
+        <v>1305</v>
       </c>
-      <c r="D7" s="1650" t="s">
-        <v>68</v>
+      <c r="D7" s="1677" t="s">
+        <v>1306</v>
       </c>
-      <c r="E7" s="1650" t="s">
-        <v>7338</v>
+      <c r="E7" s="1677" t="s">
+        <v>7369</v>
       </c>
-      <c r="F7" s="1650" t="s">
-        <v>70</v>
+      <c r="F7" s="1677" t="s">
+        <v>7370</v>
       </c>
-      <c r="G7" s="1650" t="s">
-        <v>71</v>
+      <c r="G7" s="1677" t="s">
+        <v>7371</v>
       </c>
-      <c r="H7" s="1650" t="s">
-        <v>53</v>
+      <c r="H7" s="1677" t="s">
+        <v>1309</v>
       </c>
-      <c r="I7" s="1650" t="s">
-        <v>8</v>
+      <c r="I7" s="1677" t="s">
+        <v>7372</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1651" t="s">
-        <v>72</v>
+      <c r="J7" s="1677" t="s">
+        <v>7373</v>
       </c>
-      <c r="B8" s="1651" t="s">
-        <v>72</v>
+      <c r="K7" s="1677" t="s">
+        <v>7350</v>
       </c>
-      <c r="C8" s="1651" t="s">
-        <v>7339</v>
-      </c>
-      <c r="D8" s="1651" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="1651" t="s">
-        <v>7340</v>
-      </c>
-      <c r="F8" s="1651" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="1651" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="1651" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="1651" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1652" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="1652" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="1652" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="1652" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="1652" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="1652" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="1652" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="1652" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="1652" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1653" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="1653" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="1653" t="s">
-        <v>7341</v>
-      </c>
-      <c r="D10" s="1653" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="1653" t="s">
-        <v>7342</v>
-      </c>
-      <c r="F10" s="1653" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="1653" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="1653" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="1653" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1654" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="1654" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="1654" t="s">
-        <v>7343</v>
-      </c>
-      <c r="D11" s="1654" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" s="1654" t="s">
-        <v>7344</v>
-      </c>
-      <c r="F11" s="1654" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="1654" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="1654" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" s="1654" t="s">
+      <c r="L7" s="1677" t="s">
         <v>8</v>
       </c>
     </row>
@@ -29182,7 +29468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -29190,131 +29476,188 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="73.765625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="73.765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="52.13671875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="98.4296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="25.5859375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="43.875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="28.34765625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="126.71484375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="166.87890625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="24.1796875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="13.69921875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="13.95703125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="10.87109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.87109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1655" t="s">
+      <c r="A1" s="1678" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1655" t="s">
+      <c r="B1" s="1678" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1655" t="s">
+      <c r="C1" s="1678" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1655" t="s">
+      <c r="D1" s="1678" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1655" t="s">
-        <v>9</v>
+      <c r="E1" s="1678" t="s">
+        <v>26</v>
       </c>
-      <c r="F1" s="1655" t="s">
+      <c r="F1" s="1678" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1655" t="s">
+      <c r="G1" s="1678" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1655" t="s">
+      <c r="H1" s="1678" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1655" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1655" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1655" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1655" t="s">
+      <c r="I1" s="1678" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1656" t="s">
-        <v>13</v>
+      <c r="A2" s="1679" t="s">
+        <v>27</v>
       </c>
-      <c r="B2" s="1656" t="s">
-        <v>13</v>
+      <c r="B2" s="1679" t="s">
+        <v>27</v>
       </c>
-      <c r="C2" s="1656" t="s">
-        <v>14</v>
+      <c r="C2" s="1679" t="s">
+        <v>7329</v>
       </c>
-      <c r="D2" s="1656" t="s">
-        <v>15</v>
+      <c r="D2" s="1679" t="s">
+        <v>29</v>
       </c>
-      <c r="E2" s="1656" t="s">
-        <v>1267</v>
+      <c r="E2" s="1679" t="s">
+        <v>7374</v>
       </c>
-      <c r="F2" s="1656" t="s">
-        <v>1268</v>
+      <c r="F2" s="1679" t="s">
+        <v>31</v>
       </c>
-      <c r="G2" s="1656" t="s">
-        <v>7345</v>
+      <c r="G2" s="1679" t="s">
+        <v>32</v>
       </c>
-      <c r="H2" s="1656" t="s">
-        <v>17</v>
+      <c r="H2" s="1679" t="s">
+        <v>33</v>
       </c>
-      <c r="I2" s="1656" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1656" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="1656" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="1656" t="s">
+      <c r="I2" s="1679" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1657" t="s">
-        <v>20</v>
+      <c r="A3" s="1680" t="s">
+        <v>34</v>
       </c>
-      <c r="B3" s="1657" t="s">
-        <v>20</v>
+      <c r="B3" s="1680" t="s">
+        <v>34</v>
       </c>
-      <c r="C3" s="1657" t="s">
-        <v>21</v>
+      <c r="C3" s="1680" t="s">
+        <v>35</v>
       </c>
-      <c r="D3" s="1657" t="s">
-        <v>22</v>
+      <c r="D3" s="1680" t="s">
+        <v>36</v>
       </c>
-      <c r="E3" s="1657" t="s">
-        <v>1269</v>
+      <c r="E3" s="1680" t="s">
+        <v>7375</v>
       </c>
-      <c r="F3" s="1657" t="s">
-        <v>1270</v>
+      <c r="F3" s="1680" t="s">
+        <v>7376</v>
       </c>
-      <c r="G3" s="1657" t="s">
-        <v>7346</v>
+      <c r="G3" s="1680" t="s">
+        <v>39</v>
       </c>
-      <c r="H3" s="1657" t="s">
-        <v>17</v>
+      <c r="H3" s="1680" t="s">
+        <v>33</v>
       </c>
-      <c r="I3" s="1657" t="s">
-        <v>24</v>
+      <c r="I3" s="1680" t="s">
+        <v>41</v>
       </c>
-      <c r="J3" s="1657" t="s">
-        <v>25</v>
+    </row>
+    <row r="4">
+      <c r="A4" s="1681" t="s">
+        <v>47</v>
       </c>
-      <c r="K3" s="1657" t="s">
-        <v>43</v>
+      <c r="B4" s="1681" t="s">
+        <v>47</v>
       </c>
-      <c r="L3" s="1657" t="s">
+      <c r="C4" s="1681" t="s">
+        <v>7331</v>
+      </c>
+      <c r="D4" s="1681" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="1681" t="s">
+        <v>7377</v>
+      </c>
+      <c r="F4" s="1681" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1681" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="1681" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="1681" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1682" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="1682" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1682" t="s">
+        <v>7333</v>
+      </c>
+      <c r="D5" s="1682" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="1682" t="s">
+        <v>7378</v>
+      </c>
+      <c r="F5" s="1682" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="1682" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="1682" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="1682" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1683" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="1683" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1683" t="s">
+        <v>7335</v>
+      </c>
+      <c r="D6" s="1683" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="1683" t="s">
+        <v>7379</v>
+      </c>
+      <c r="F6" s="1683" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="1683" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="1683" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="1683" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented some missing steps
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="BrandItemPageData" sheetId="46" r:id="rId2"/>
-    <sheet name="BrandPageData" sheetId="47" r:id="rId3"/>
+    <sheet name="BrandItemPageData" sheetId="48" r:id="rId2"/>
+    <sheet name="BrandPageData" sheetId="49" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -457,7 +457,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added the items tests steps
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="BrandItemPageData" sheetId="48" r:id="rId2"/>
-    <sheet name="BrandPageData" sheetId="49" r:id="rId3"/>
+    <sheet name="BrandItemPageData" sheetId="52" r:id="rId2"/>
+    <sheet name="BrandPageData" sheetId="53" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -130,13 +130,223 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,23 +664,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="73.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="52.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="98.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="100.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="79.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="125.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="255" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="126.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="166.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="198.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="248.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="141.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -513,6 +723,706 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="38"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="41"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="41"/>
+      <c r="L41" s="41"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="42"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="45"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="47"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="48"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="48"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="49"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
+      <c r="J49" s="49"/>
+      <c r="K49" s="49"/>
+      <c r="L49" s="49"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="50"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -520,52 +1430,272 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A2" sqref="A2:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="143.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="71.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="145.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="255" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="81.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="126.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="178.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="52" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="56"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="60"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="63"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="65"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="66"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="68"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="69"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="71"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="72"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>